<commit_message>
output processing params. removed temp indexed table
</commit_message>
<xml_diff>
--- a/examples/table_annotation/table_ANNOTATED.xlsx
+++ b/examples/table_annotation/table_ANNOTATED.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,57 +476,52 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Vertebrata_best mean z-score over 5 residue window</t>
+          <t>Tetrapoda_conservation_string</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Tetrapoda_conservation_string</t>
+          <t>Tetrapoda_aln_slice_file</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Tetrapoda_aln_slice_file</t>
+          <t>Tetrapoda_hit_mean_zscore</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Tetrapoda_hit_mean_zscore</t>
+          <t>json_file</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Tetrapoda_best mean z-score over 5 residue window</t>
+          <t>multi_level_plot</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>json_file</t>
+          <t>hit_start_position</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>multi_level_plot</t>
+          <t>regex</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>hit_start_position</t>
+          <t>regex_match</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>regex</t>
+          <t>Vertebrata_regex_match_mean_zscore</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>regex_match</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>regex_match_stpos_in_hit</t>
+          <t>Tetrapoda_regex_match_mean_zscore</t>
         </is>
       </c>
     </row>
@@ -563,7 +558,6 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -598,7 +592,6 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -632,48 +625,45 @@
       <c r="H4" t="n">
         <v>-0.9222526690491762</v>
       </c>
-      <c r="I4" t="n">
-        <v>-0.2700237567408307</v>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>___P_______</t>
         </is>
       </c>
-      <c r="K4">
+      <c r="J4">
         <f>HYPERLINK("conservation_analysis/2-9606_0_002f40/2-9606_0002f40-Tetrapoda_aln_slice.html")</f>
         <v/>
       </c>
-      <c r="L4" t="n">
+      <c r="K4" t="n">
         <v>-0.5883645445360336</v>
       </c>
-      <c r="M4" t="n">
-        <v>0.007553186685062716</v>
-      </c>
-      <c r="N4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>/Users/jackson/Dropbox (MIT)/work/07-SLiM_bioinformatics/05-conservation_pipeline/examples/table_annotation/conservation_analysis/2-9606_0_002f40/2-9606_0_002f40.json</t>
         </is>
       </c>
-      <c r="O4">
+      <c r="M4">
         <f>HYPERLINK("./conservation_analysis/2-9606_0_002f40/2-9606_0002f40-aln_property_entropy_og_level_score_screen.png")</f>
         <v/>
       </c>
-      <c r="P4" t="n">
+      <c r="N4" t="n">
         <v>259</v>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>P.P.E</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>PNPEE</t>
         </is>
       </c>
-      <c r="S4" t="n">
-        <v>3</v>
+      <c r="Q4" t="n">
+        <v>-0.7300460456318796</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-0.3685849517941594</v>
       </c>
     </row>
     <row r="5">
@@ -708,43 +698,38 @@
       <c r="H5" t="n">
         <v>-1.112491301468793</v>
       </c>
-      <c r="I5" t="n">
-        <v>-0.07523790268240245</v>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>_______E____</t>
         </is>
       </c>
-      <c r="K5">
+      <c r="J5">
         <f>HYPERLINK("conservation_analysis/3-9606_0_002f40/3-9606_0002f40-Tetrapoda_aln_slice.html")</f>
         <v/>
       </c>
-      <c r="L5" t="n">
+      <c r="K5" t="n">
         <v>-0.9654074901111241</v>
       </c>
-      <c r="M5" t="n">
-        <v>0.2974683718419012</v>
-      </c>
-      <c r="N5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>/Users/jackson/Dropbox (MIT)/work/07-SLiM_bioinformatics/05-conservation_pipeline/examples/table_annotation/conservation_analysis/3-9606_0_002f40/3-9606_0_002f40.json</t>
         </is>
       </c>
-      <c r="O5">
+      <c r="M5">
         <f>HYPERLINK("./conservation_analysis/3-9606_0_002f40/3-9606_0002f40-aln_property_entropy_og_level_score_screen.png")</f>
         <v/>
       </c>
-      <c r="P5" t="n">
+      <c r="N5" t="n">
         <v>302</v>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>P.P.E</t>
         </is>
       </c>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -783,7 +768,6 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -822,7 +806,6 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -861,7 +844,6 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>